<commit_message>
I Aint Building That 업데이트
#340
</commit_message>
<xml_diff>
--- a/Data/I Aint Building That - 3118060751/3118060751.xlsx
+++ b/Data/I Aint Building That - 3118060751/3118060751.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\default\I Aint Building That - 3118060751\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\I Aint Building That - 3118060751\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062F56D1-2CE4-4195-8C9A-AC54029A4952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529B9B8D-203F-416D-BA32-73FF6C76761D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_231223" sheetId="2" r:id="rId1"/>
+    <sheet name="231221" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -79,6 +80,21 @@
   </si>
   <si>
     <t>Taggerung.IAintBuildingThat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keyed+Taggerung_IAintBuildingThat_SearchLabel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taggerung_IAintBuildingThat_SearchLabel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>필터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -449,10 +465,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6D2C18-2A01-47B2-83D6-157B4224F88C}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>